<commit_message>
full data from 2000
</commit_message>
<xml_diff>
--- a/capiq_data/in_process_data/IQ112732.xlsx
+++ b/capiq_data/in_process_data/IQ112732.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yedid\Desktop\capiq_3\in_process_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yedid\Desktop\credit_rating_predictions-main\capiq_data\in_process_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B534B7D1-0630-460C-A50D-720613DC3485}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3964EDD-1836-48F1-A484-7A3AED294B81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="98" windowWidth="14400" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"fe89273d-ff52-42bb-9138-0724ae734bfd"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"dfa706d0-53ba-4742-bf9f-4cb1a109421b"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.45.614.5792"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -41,7 +41,7 @@
     <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
     <definedName name="IQ_MONTH">15000</definedName>
     <definedName name="IQ_MTD" hidden="1">800000</definedName>
-    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">44257.9003703704</definedName>
+    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">44278.8607986111</definedName>
     <definedName name="IQ_NTM">6000</definedName>
     <definedName name="IQ_QTD" hidden="1">750000</definedName>
     <definedName name="IQ_TODAY" hidden="1">0</definedName>

</xml_diff>